<commit_message>
Update parameteres for v0.2A in Example data folder
</commit_message>
<xml_diff>
--- a/Example_Data/Tarland_Scotland/Parameters_v0-2A_Tarland.xlsx
+++ b/Example_Data/Tarland_Scotland/Parameters_v0-2A_Tarland.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\SimplyP\Development\v0-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\SimplyP\Current_Release\v0-2A\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="690" windowWidth="18198" windowHeight="11160" tabRatio="649" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="690" windowWidth="18198" windowHeight="11160" tabRatio="649"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="8" r:id="rId1"/>
@@ -598,9 +598,6 @@
     <t>Bulk density(kg/m3)</t>
   </si>
   <si>
-    <t>C:\Data\SimplyP_Local\Temp\Output</t>
-  </si>
-  <si>
     <t>Average latitude of the catchment (used in Thornthwaite PET calculation)</t>
   </si>
   <si>
@@ -689,27 +686,10 @@
 Values can be sourced from (R)USLE literature. Differences in inherent soil erodibility are generally termed the K factor in USLE-related literature.</t>
   </si>
   <si>
-    <t>C:\Data\GitHub\SimplyP\Example_Data\Tarland_Scotland\Tarland_MetData_1981-2010.csv</t>
-  </si>
-  <si>
-    <t>C:\Data\GitHub\SimplyP\Example_Data\Tarland_Scotland\Observations\Coull_ChemObs.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Data\GitHub\SimplyP\Example_Data\Tarland_Scotland\Observations\Coull_DailyMeanQ.xlsx</t>
-  </si>
-  <si>
-    <t>Q, TDP, PP</t>
-  </si>
-  <si>
     <t>2004-01-01</t>
   </si>
   <si>
     <t>2004-12-31</t>
-  </si>
-  <si>
-    <t>One of 'cal', 'other'. Determines:
-- whether Kf is calculated (calibration period) or read in
-- whether observations are plotted (only done for cal &amp; val only)</t>
   </si>
   <si>
     <t>Simulation end date. If calculating PET, must be near 31st December of given year</t>
@@ -737,10 +717,6 @@
 Semi-natural fixed at 0. NC automatically assigned within model</t>
   </si>
   <si>
-    <t>Only supply a value for A.
-Semi-natural fixed at 0. Newly-converted value could be negative if have net uptake and removal</t>
-  </si>
-  <si>
     <t>Proportion of semi-natural and other low soil-P land (value in range 0-1)</t>
   </si>
   <si>
@@ -765,9 +741,6 @@
     <t>Reach effluent TDP inputs. In-stream retention and re-release is not currently taken into account in the model, so if this is important in your catchment you may need to consider this parameter as net inputs after retention</t>
   </si>
   <si>
-    <t>Set to 1 unless PET thought to be systematically under or over-estimated by Thornthwaite in the study area</t>
-  </si>
-  <si>
     <t>Baseflow index (proportion of soil water flow that percolates to groundwater vs flowing to the reach)</t>
   </si>
   <si>
@@ -832,6 +805,33 @@
   </si>
   <si>
     <t>Choose from: SS, TDP, PP, TP, Q, SRP (in any order)</t>
+  </si>
+  <si>
+    <t>..\..\Example_Data\Tarland_Scotland\Tarland_MetData_1981-2010.csv</t>
+  </si>
+  <si>
+    <t>..\..\Example_Data\Tarland_Scotland\Observations\Coull_ChemObs.xlsx</t>
+  </si>
+  <si>
+    <t>..\..\Example_Data\Tarland_Scotland\Observations\Coull_DailyMeanQ.xlsx</t>
+  </si>
+  <si>
+    <t>..\..\Example_Data\Example_Output</t>
+  </si>
+  <si>
+    <t>One of 'cal', 'val' or 'scenario'. Determines:
+- whether Kf is calculated (calibration period) or read in. If the latter, then a value for Kf must be supplied in the 'Constant' sheet. This is obtained from calibration.
+- whether observations are plotted (only for cal &amp; val)
+- goodness of fit stats only calculated if not 'scenario'</t>
+  </si>
+  <si>
+    <t>SS, TDP, PP, TP, Q, SRP</t>
+  </si>
+  <si>
+    <t>Only supply a value for A and newly-converted (NC) if any NC land present. Semi-natural fixed at 0. Newly-converted value could be negative if have net uptake and removal</t>
+  </si>
+  <si>
+    <t>Set to 1 unless PET thought to be systematically under or over-estimated in the study area</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1689,6 +1689,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2539,7 +2545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
@@ -2554,17 +2560,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="21.578125" style="20" customWidth="1"/>
     <col min="2" max="2" width="55.41796875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="31.3671875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="31.3125" style="20" customWidth="1"/>
     <col min="4" max="4" width="47.41796875" style="20" customWidth="1"/>
-    <col min="5" max="16384" width="9.15625" style="20"/>
+    <col min="5" max="16384" width="9.1015625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2589,7 +2595,7 @@
         <v>92</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>113</v>
@@ -2600,16 +2606,16 @@
         <v>93</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>113</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2617,16 +2623,16 @@
         <v>94</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>113</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2637,18 +2643,18 @@
         <v>116</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>179</v>
+        <v>251</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>215</v>
+        <v>252</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>176</v>
@@ -2676,10 +2682,10 @@
         <v>96</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>112</v>
@@ -2690,21 +2696,21 @@
         <v>97</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="26" t="s">
         <v>98</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C10" s="20">
         <v>1</v>
@@ -2718,10 +2724,10 @@
         <v>99</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>114</v>
@@ -2743,25 +2749,25 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>190</v>
-      </c>
       <c r="C13" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" s="30"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14" s="30"/>
     </row>
@@ -2773,7 +2779,7 @@
         <v>143</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>114</v>
@@ -2787,7 +2793,7 @@
         <v>141</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>114</v>
@@ -2798,7 +2804,7 @@
         <v>131</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>103</v>
@@ -2868,13 +2874,13 @@
         <v>132</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>202</v>
-      </c>
       <c r="D22" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2885,10 +2891,10 @@
         <v>122</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>212</v>
+        <v>253</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2927,10 +2933,10 @@
         <v>146</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2944,7 +2950,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2956,13 +2962,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="139" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B1" s="139" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C1" s="139" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2982,18 +2988,18 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.15625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.68359375" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.15625" style="17"/>
+    <col min="3" max="3" width="9.1015625" style="17"/>
     <col min="4" max="4" width="61.7890625" style="17" customWidth="1"/>
-    <col min="5" max="8" width="9.15625" style="17"/>
-    <col min="9" max="9" width="51.15625" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="9.15625" style="17"/>
+    <col min="5" max="8" width="9.1015625" style="17"/>
+    <col min="9" max="9" width="51.1015625" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.1015625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3047,7 +3053,7 @@
       <c r="G2" s="70"/>
       <c r="H2" s="71"/>
       <c r="I2" s="97" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -3061,7 +3067,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E3" s="135">
         <v>1458</v>
@@ -3072,7 +3078,7 @@
       <c r="G3" s="76"/>
       <c r="H3" s="77"/>
       <c r="I3" s="98" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -3086,7 +3092,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E4" s="137">
         <v>10</v>
@@ -3096,13 +3102,13 @@
       </c>
       <c r="G4" s="83"/>
       <c r="H4" s="84">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="I4" s="99" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="78" customFormat="1" ht="61.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="78" customFormat="1" ht="61.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="85" t="s">
         <v>150</v>
       </c>
@@ -3113,7 +3119,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E5" s="138">
         <v>0.1</v>
@@ -3124,7 +3130,7 @@
       <c r="G5" s="89"/>
       <c r="H5" s="90"/>
       <c r="I5" s="100" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="95" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -3138,7 +3144,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E6" s="91">
         <v>0.2</v>
@@ -3151,7 +3157,7 @@
       </c>
       <c r="H6" s="94"/>
       <c r="I6" s="101" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="172" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -3165,7 +3171,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="175" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E7" s="173">
         <v>0</v>
@@ -3178,7 +3184,7 @@
       </c>
       <c r="H7" s="96"/>
       <c r="I7" s="176" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3191,16 +3197,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.15625" style="144" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1015625" style="144" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83984375" style="144" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.83984375" style="144"/>
-    <col min="4" max="4" width="58.89453125" style="144" customWidth="1"/>
+    <col min="4" max="4" width="58.83984375" style="144" customWidth="1"/>
     <col min="5" max="16384" width="8.83984375" style="144"/>
   </cols>
   <sheetData>
@@ -3249,7 +3255,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="146" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E3" s="147">
         <v>0.2</v>
@@ -3266,7 +3272,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="146" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E4" s="147">
         <v>0.3</v>
@@ -3283,7 +3289,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="146" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E5" s="147">
         <v>0.5</v>
@@ -3300,7 +3306,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="179" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E6" s="180">
         <v>0</v>
@@ -3317,7 +3323,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="179" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E7" s="180">
         <v>0</v>
@@ -3334,26 +3340,26 @@
         <v>17</v>
       </c>
       <c r="D8" s="179" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E8" s="180">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="92" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="92" t="s">
+    <row r="9" spans="1:5" s="197" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="197" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="197" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="197" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="93" t="s">
-        <v>231</v>
-      </c>
-      <c r="E9" s="147">
+      <c r="D9" s="198" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" s="180">
         <v>0.65</v>
       </c>
     </row>
@@ -3453,7 +3459,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E15" s="151">
         <v>0.1</v>
@@ -3469,19 +3475,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1015625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.68359375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.15625" style="5"/>
+    <col min="3" max="3" width="9.1015625" style="5"/>
     <col min="4" max="4" width="64.5234375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.15625" style="5"/>
+    <col min="5" max="5" width="9.1015625" style="5"/>
     <col min="6" max="6" width="62.3125" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.15625" style="5"/>
+    <col min="7" max="16384" width="9.1015625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3521,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="184" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3541,7 +3547,7 @@
         <v>2.74</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3549,19 +3555,19 @@
         <v>61</v>
       </c>
       <c r="B4" s="182" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" s="182" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="183" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E4" s="182">
         <v>59.596699999999998</v>
       </c>
       <c r="F4" s="184" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3575,7 +3581,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="153" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E5" s="141">
         <v>0.02</v>
@@ -3593,13 +3599,13 @@
         <v>17</v>
       </c>
       <c r="D6" s="154" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E6" s="171">
         <v>1</v>
       </c>
       <c r="F6" s="117" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3613,13 +3619,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="153" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E7" s="140">
         <v>290</v>
       </c>
       <c r="F7" s="49" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3633,7 +3639,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="153" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E8" s="141">
         <v>0.7</v>
@@ -3675,7 +3681,7 @@
         <v>0.4</v>
       </c>
       <c r="F10" s="49" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3695,7 +3701,7 @@
         <v>0.5</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3715,7 +3721,7 @@
         <v>0.42</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3729,13 +3735,13 @@
         <v>52</v>
       </c>
       <c r="D13" s="153" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E13" s="132">
         <v>1</v>
       </c>
       <c r="F13" s="188" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="G13" s="114"/>
     </row>
@@ -3744,25 +3750,25 @@
         <v>61</v>
       </c>
       <c r="B14" s="120" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="120" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="156" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E14" s="121">
         <v>1</v>
       </c>
       <c r="F14" s="122" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G14" s="123"/>
     </row>
     <row r="15" spans="1:7" s="128" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="125" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B15" s="126" t="s">
         <v>32</v>
@@ -3771,18 +3777,18 @@
         <v>53</v>
       </c>
       <c r="D15" s="157" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E15" s="161">
         <v>95</v>
       </c>
       <c r="F15" s="127" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="128" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="129" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B16" s="130" t="s">
         <v>9</v>
@@ -3791,18 +3797,18 @@
         <v>59</v>
       </c>
       <c r="D16" s="158" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E16" s="162">
         <v>1.1315280460000001E-4</v>
       </c>
       <c r="F16" s="131" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="189" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B17" s="190" t="s">
         <v>30</v>
@@ -3820,27 +3826,27 @@
     </row>
     <row r="18" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="189" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B18" s="190" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="190" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="163" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E18" s="165">
         <v>0.7</v>
       </c>
       <c r="F18" s="164" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="192" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="196" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B19" s="193" t="s">
         <v>31</v>
@@ -3849,7 +3855,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="194" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E19" s="195">
         <v>1.6</v>
@@ -3867,7 +3873,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="159" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E20" s="142">
         <v>1500</v>
@@ -3885,7 +3891,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="159" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E21" s="169">
         <v>2</v>
@@ -3909,7 +3915,7 @@
         <v>60</v>
       </c>
       <c r="F22" s="170" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3946,7 +3952,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="16.26171875" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
@@ -3956,7 +3962,7 @@
     <col min="6" max="6" width="78.41796875" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.83984375" style="2" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.15625" style="2"/>
+    <col min="9" max="16384" width="9.1015625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">

</xml_diff>